<commit_message>
POB, debt, eehc, pension changes
</commit_message>
<xml_diff>
--- a/funds_ab_in_2022.xlsx
+++ b/funds_ab_in_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Desktop\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Desktop\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Replication-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443DF5B0-F093-4A3B-8A7C-EA2A0BEF8120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B011CECD-7E01-4E06-8B6B-493144962E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6814" uniqueCount="2508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6815" uniqueCount="2508">
   <si>
     <t>fund</t>
   </si>
@@ -7732,25 +7732,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -7806,6 +7787,25 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7820,18 +7820,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92861C71-2608-406B-AB38-61A950AD4A6E}" name="Table1" displayName="Table1" ref="A1:K1104" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92861C71-2608-406B-AB38-61A950AD4A6E}" name="Table1" displayName="Table1" ref="A1:K1104" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K1104" xr:uid="{92861C71-2608-406B-AB38-61A950AD4A6E}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5C12AE88-F5C0-4F1D-BC84-FFCA81419500}" name="fund" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{CEDB1617-12CC-4191-B126-9922068A1353}" name="fund_ab" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{4C1E1072-690E-4905-AD33-33117D00B670}" name="fund_ioc" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{57A480F5-EA3F-465F-975E-2A2B1C7302FA}" name="fund_re" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{5C244DC3-32C4-4224-BC6D-7AE06CED4898}" name="a_end" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{8464D253-7DFF-48A9-878F-3C3F48DA8414}" name="in_ff" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{ECBCF6D7-D1E8-4215-AAC1-21E353589401}" name="fund_name_ab" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{43B46110-966C-42D4-BE04-99C9CB9FACD9}" name="fund_category" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{DAF8ADA5-8C0F-4603-BF33-F6FD7A1BE6F8}" name="fund_cat_name" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{5C12AE88-F5C0-4F1D-BC84-FFCA81419500}" name="fund" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{CEDB1617-12CC-4191-B126-9922068A1353}" name="fund_ab" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4C1E1072-690E-4905-AD33-33117D00B670}" name="fund_ioc" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{57A480F5-EA3F-465F-975E-2A2B1C7302FA}" name="fund_re" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5C244DC3-32C4-4224-BC6D-7AE06CED4898}" name="a_end" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{8464D253-7DFF-48A9-878F-3C3F48DA8414}" name="in_ff" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{ECBCF6D7-D1E8-4215-AAC1-21E353589401}" name="fund_name_ab" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{43B46110-966C-42D4-BE04-99C9CB9FACD9}" name="fund_category" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{DAF8ADA5-8C0F-4603-BF33-F6FD7A1BE6F8}" name="fund_cat_name" dataDxfId="2"/>
     <tableColumn id="12" xr3:uid="{5D37F4FD-4156-43F6-9EBC-23D0DE526378}" name="in_ff_rev" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{712C439E-EFDF-45F0-B386-D57653FB61D3}" name="in_ff_exp" dataDxfId="0"/>
   </tableColumns>
@@ -8163,8 +8163,8 @@
   <dimension ref="A1:K1104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1087" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1012" sqref="H1012"/>
+      <pane ySplit="1" topLeftCell="A802" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G817" sqref="G817"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35112,8 +35112,8 @@
         <v>0</v>
       </c>
       <c r="E817" s="2"/>
-      <c r="F817" s="2">
-        <v>1</v>
+      <c r="F817" s="2" t="s">
+        <v>2369</v>
       </c>
       <c r="G817" s="1" t="s">
         <v>2030</v>

</xml_diff>

<commit_message>
Deleted old lines of code. Edited pension obligations and included pension stabilization fund in analysis
</commit_message>
<xml_diff>
--- a/funds_ab_in_2022.xlsx
+++ b/funds_ab_in_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Desktop\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Replication-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Replication-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B210A92-E73C-4BBB-9986-6779D3D9764F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5088C4-ADB2-43F6-8E77-37C19B8155EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="366" yWindow="366" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -8188,8 +8188,8 @@
   <dimension ref="A1:K1105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1090" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1069" sqref="C1069"/>
+      <pane ySplit="1" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K359" sqref="K359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20139,8 +20139,8 @@
         <v>2369</v>
       </c>
       <c r="E359" s="2"/>
-      <c r="F359" s="2" t="s">
-        <v>2369</v>
+      <c r="F359" s="18" t="s">
+        <v>2319</v>
       </c>
       <c r="G359" s="1" t="s">
         <v>2442</v>
@@ -20151,11 +20151,11 @@
       <c r="I359" s="1" t="s">
         <v>2289</v>
       </c>
-      <c r="J359" s="1" t="s">
-        <v>2369</v>
-      </c>
-      <c r="K359" s="1" t="s">
-        <v>2369</v>
+      <c r="J359" s="3" t="s">
+        <v>2319</v>
+      </c>
+      <c r="K359" s="3" t="s">
+        <v>2319</v>
       </c>
     </row>
     <row r="360" spans="1:11">

</xml_diff>

<commit_message>
Changed TOC order. Cleaned up comments throughout code.
</commit_message>
<xml_diff>
--- a/funds_ab_in_2022.xlsx
+++ b/funds_ab_in_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Replication-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5088C4-ADB2-43F6-8E77-37C19B8155EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62566AE9-0A2A-4B99-B8A8-B7DC8903716A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8188,8 +8188,8 @@
   <dimension ref="A1:K1105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K359" sqref="K359"/>
+      <pane ySplit="1" topLeftCell="A919" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F925" sqref="F925"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -38915,7 +38915,7 @@
       </c>
       <c r="E924" s="2"/>
       <c r="F924" s="2" t="s">
-        <v>2369</v>
+        <v>2319</v>
       </c>
       <c r="G924" s="13" t="s">
         <v>2030</v>

</xml_diff>

<commit_message>
Updated tables, column names, graphs, cleaned up document.
</commit_message>
<xml_diff>
--- a/funds_ab_in_2022.xlsx
+++ b/funds_ab_in_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures FY2022\Replication-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FF8F8B-5F47-443F-8E3B-FE538ED0E8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901C51DE-FB4A-429F-9DB3-691BC2680200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2652" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14100" yWindow="-16200" windowWidth="29070" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -8180,7 +8180,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A356" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F367" sqref="F367"/>
+      <selection pane="bottomLeft" activeCell="G366" sqref="G366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20398,7 +20398,7 @@
         <v>2316</v>
       </c>
       <c r="E367" s="1"/>
-      <c r="F367" s="1" t="s">
+      <c r="F367" s="2" t="s">
         <v>2319</v>
       </c>
       <c r="G367" s="1" t="s">

</xml_diff>